<commit_message>
updates in BOM gerber and PCL
</commit_message>
<xml_diff>
--- a/BOM/BIM_PCB.xlsx
+++ b/BOM/BIM_PCB.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\kicad6\KICAD 6.0.0\contractual_projects\ECO_BODA\BIM_PCB\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D57719D6-78E4-4532-8D2B-DA80AEFF3452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB2B8825-40EC-47DB-BC52-C8D82DF0E15B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="383" uniqueCount="238">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="281" uniqueCount="223">
   <si>
     <t>Qty</t>
   </si>
@@ -42,6 +42,9 @@
     <t>MPN</t>
   </si>
   <si>
+    <t>AE1, AE2</t>
+  </si>
+  <si>
     <t>Antenna_Shield</t>
   </si>
   <si>
@@ -57,63 +60,72 @@
     <t>Battery:BatteryHolder_LINX_BAT-HLD-012-SMT</t>
   </si>
   <si>
+    <t>C1, C2, C3, C4, C5, C7, C8, C24, C25, C30, C31, C33, C34, C39, C40, C41, C43, C44, C49, C50, C52</t>
+  </si>
+  <si>
     <t>100n</t>
   </si>
   <si>
     <t>Capacitor_SMD:C_0402_1005Metric</t>
   </si>
   <si>
+    <t>C6, C23, C29</t>
+  </si>
+  <si>
     <t>1u</t>
   </si>
   <si>
+    <t>C9, C10, C11, C12, C18, C19, C20</t>
+  </si>
+  <si>
     <t>22p</t>
   </si>
   <si>
+    <t>C13, C26, C27, C32, C42, C51</t>
+  </si>
+  <si>
     <t>10u</t>
   </si>
   <si>
-    <t>C14</t>
-  </si>
-  <si>
-    <t>0.3p</t>
-  </si>
-  <si>
-    <t>C20</t>
-  </si>
-  <si>
-    <t>1000u</t>
-  </si>
-  <si>
-    <t>Capacitor_Tantalum_SMD:CP_EIA-7343-43_Kemet-X</t>
-  </si>
-  <si>
-    <t>T491X108K006AT</t>
-  </si>
-  <si>
-    <t>C22</t>
+    <t>C14, C16, C21</t>
+  </si>
+  <si>
+    <t>0.1u</t>
+  </si>
+  <si>
+    <t>C15, C17, C22</t>
+  </si>
+  <si>
+    <t>C28</t>
+  </si>
+  <si>
+    <t>100u</t>
+  </si>
+  <si>
+    <t>Capacitor_Tantalum_SMD:CP_EIA-3216-18_Kemet-A</t>
+  </si>
+  <si>
+    <t>TLJA107M006R0800</t>
+  </si>
+  <si>
+    <t>C46, C58</t>
+  </si>
+  <si>
+    <t>Capacitor_SMD:C_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>C47</t>
+  </si>
+  <si>
+    <t>8.2p</t>
+  </si>
+  <si>
+    <t>C48</t>
   </si>
   <si>
     <t>10n</t>
   </si>
   <si>
-    <t>C23</t>
-  </si>
-  <si>
-    <t>1n</t>
-  </si>
-  <si>
-    <t>Capacitor_SMD:C_0603_1608Metric</t>
-  </si>
-  <si>
-    <t>C47</t>
-  </si>
-  <si>
-    <t>8.2p</t>
-  </si>
-  <si>
-    <t>C48</t>
-  </si>
-  <si>
     <t>C53</t>
   </si>
   <si>
@@ -132,6 +144,9 @@
     <t>22u</t>
   </si>
   <si>
+    <t>C56, C57</t>
+  </si>
+  <si>
     <t>D1</t>
   </si>
   <si>
@@ -162,79 +177,136 @@
     <t>D4</t>
   </si>
   <si>
+    <t>SP0504BAHT</t>
+  </si>
+  <si>
+    <t>Package_TO_SOT_SMD:SOT-23-5</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
     <t>ORANGE</t>
   </si>
   <si>
-    <t>D5</t>
+    <t>D6</t>
   </si>
   <si>
     <t>BLUE</t>
   </si>
   <si>
-    <t>D6</t>
-  </si>
-  <si>
-    <t>SP0504BAHT</t>
-  </si>
-  <si>
-    <t>Package_TO_SOT_SMD:SOT-23-5</t>
+    <t>D7, D8, D13, D14, D16, D17</t>
   </si>
   <si>
     <t>BEP0080MA</t>
   </si>
   <si>
+    <t>D9, D15, D18</t>
+  </si>
+  <si>
     <t>ESDONCAN1LT1G</t>
   </si>
   <si>
     <t>Package_TO_SOT_SMD:SOT-23</t>
   </si>
   <si>
+    <t>D10, D11, D12</t>
+  </si>
+  <si>
     <t>SS310</t>
   </si>
   <si>
     <t>Diode_SMD:D_SMA</t>
   </si>
   <si>
-    <t>FL1</t>
-  </si>
-  <si>
-    <t>B39162B8813P810</t>
-  </si>
-  <si>
-    <t>Filter:Filter_1109-5_1.1x0.9mm</t>
-  </si>
-  <si>
-    <t>Conn_02x02_Odd_Even</t>
-  </si>
-  <si>
-    <t>Connector_Molex:Molex_Nano-Fit_105314-xx04_2x02_P2.50mm_Horizontal</t>
+    <t>D+1</t>
+  </si>
+  <si>
+    <t>D+</t>
+  </si>
+  <si>
+    <t>brilliant-kicad-library:TestPoint_Pad_D0.9mm</t>
+  </si>
+  <si>
+    <t>D-1</t>
+  </si>
+  <si>
+    <t>D-</t>
+  </si>
+  <si>
+    <t>H2, H3, H4</t>
+  </si>
+  <si>
+    <t>MountingHole</t>
+  </si>
+  <si>
+    <t>MountingHole:MountingHole_2.7mm</t>
+  </si>
+  <si>
+    <t>HST_RXD1</t>
+  </si>
+  <si>
+    <t>HST_RXD</t>
+  </si>
+  <si>
+    <t>HST_TXD1</t>
+  </si>
+  <si>
+    <t>HST_TXD</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>Conn_02x09_Counter_Clockwise</t>
+  </si>
+  <si>
+    <t>Connector_Molex:Molex_Mini-Fit_Jr_5569-18A2_2x09_P4.20mm_Horizontal</t>
   </si>
   <si>
     <t>J2</t>
   </si>
   <si>
-    <t>Conn_02x03_Odd_Even</t>
-  </si>
-  <si>
-    <t>Connector_Molex:Molex_Nano-Fit_105314-xx06_2x03_P2.50mm_Horizontal</t>
+    <t>nano_sim</t>
+  </si>
+  <si>
+    <t>MACHADA_footprints:nano_sim_NSIM-2-C</t>
+  </si>
+  <si>
+    <t>NSIM-2-C</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>Conn_01x06</t>
+  </si>
+  <si>
+    <t>greencharge-footprints:J-LINK_6-PIN_NEEDLE_ADAPTER</t>
   </si>
   <si>
     <t>J4</t>
   </si>
   <si>
-    <t>DISPLAY CONNECTOR</t>
-  </si>
-  <si>
-    <t>J5</t>
-  </si>
-  <si>
-    <t>nano_sim</t>
-  </si>
-  <si>
-    <t>MACHADA_footprints:nano_sim_NSIM-2-C</t>
-  </si>
-  <si>
-    <t>NSIM-2-C</t>
+    <t>Micro_SD_Card</t>
+  </si>
+  <si>
+    <t>MACHADA_footprints:MOLEX_503398-1892</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>BOOT0</t>
+  </si>
+  <si>
+    <t>Jumper:SolderJumper-3_P1.3mm_Open_RoundedPad1.0x1.5mm_NumberLabels</t>
+  </si>
+  <si>
+    <t>JP2</t>
+  </si>
+  <si>
+    <t>BOOT1</t>
   </si>
   <si>
     <t>L1</t>
@@ -249,24 +321,12 @@
     <t>L2</t>
   </si>
   <si>
-    <t>1uH</t>
+    <t>82nH</t>
   </si>
   <si>
     <t>Inductor_SMD:L_0402_1005Metric</t>
   </si>
   <si>
-    <t>L3</t>
-  </si>
-  <si>
-    <t>100mHz 150/200R</t>
-  </si>
-  <si>
-    <t>L4</t>
-  </si>
-  <si>
-    <t>27nH</t>
-  </si>
-  <si>
     <t>L5</t>
   </si>
   <si>
@@ -279,6 +339,9 @@
     <t>MDA5030-2R2M</t>
   </si>
   <si>
+    <t>Q1, Q2</t>
+  </si>
+  <si>
     <t>SSM3J328R-HXY</t>
   </si>
   <si>
@@ -288,12 +351,18 @@
     <t>IRLML0100TRPBF</t>
   </si>
   <si>
+    <t>Q4, Q7, Q8, Q9</t>
+  </si>
+  <si>
+    <t>2N7002</t>
+  </si>
+  <si>
+    <t>Q5, Q6</t>
+  </si>
+  <si>
     <t>BSN20</t>
   </si>
   <si>
-    <t>2N7002</t>
-  </si>
-  <si>
     <t>R1</t>
   </si>
   <si>
@@ -303,9 +372,15 @@
     <t>Resistor_SMD:R_0402_1005Metric</t>
   </si>
   <si>
+    <t>R2, R5, R6, R17, R18, R48, R49, R51, R52, R54, R55, R67, R69</t>
+  </si>
+  <si>
     <t>10K</t>
   </si>
   <si>
+    <t>R3, R4, R9, R31, R32, R58, R61, R65</t>
+  </si>
+  <si>
     <t>100K</t>
   </si>
   <si>
@@ -321,72 +396,126 @@
     <t>499R</t>
   </si>
   <si>
+    <t>R10, R12, R37, R39, R62, R64</t>
+  </si>
+  <si>
     <t>10R</t>
   </si>
   <si>
+    <t>R11, R15, R38, R63</t>
+  </si>
+  <si>
     <t>220R</t>
   </si>
   <si>
+    <t>R13, R14, R16</t>
+  </si>
+  <si>
     <t>4.7K</t>
   </si>
   <si>
+    <t>R19, R50, R53, R56</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>R20, R23, R24</t>
+  </si>
+  <si>
     <t>1k</t>
   </si>
   <si>
-    <t>R18</t>
-  </si>
-  <si>
-    <t>0R</t>
-  </si>
-  <si>
-    <t>R21</t>
+    <t>R21, R22, R25</t>
+  </si>
+  <si>
+    <t>R26, R27</t>
   </si>
   <si>
     <t>2.2K</t>
   </si>
   <si>
+    <t>R28, R29, R30</t>
+  </si>
+  <si>
+    <t>22R</t>
+  </si>
+  <si>
+    <t>R33</t>
+  </si>
+  <si>
+    <t>200K</t>
+  </si>
+  <si>
+    <t>R34</t>
+  </si>
+  <si>
+    <t>R35, R36</t>
+  </si>
+  <si>
+    <t>390R</t>
+  </si>
+  <si>
+    <t>R40, R41, R42, R45, R46, R47</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>R43, R44, R59, R60</t>
+  </si>
+  <si>
+    <t>60R</t>
+  </si>
+  <si>
+    <t>R66</t>
+  </si>
+  <si>
+    <t>R68</t>
+  </si>
+  <si>
+    <t>100R</t>
+  </si>
+  <si>
+    <t>R70</t>
+  </si>
+  <si>
+    <t>180K</t>
+  </si>
+  <si>
+    <t>RC0402FR-07180KL</t>
+  </si>
+  <si>
+    <t>R71</t>
+  </si>
+  <si>
+    <t>40K</t>
+  </si>
+  <si>
     <t>Resistor_SMD:R_0603_1608Metric</t>
   </si>
   <si>
-    <t>390R</t>
-  </si>
-  <si>
-    <t>22R</t>
-  </si>
-  <si>
-    <t>1K</t>
-  </si>
-  <si>
-    <t>60R</t>
-  </si>
-  <si>
-    <t>R66</t>
-  </si>
-  <si>
-    <t>R68</t>
-  </si>
-  <si>
-    <t>100R</t>
-  </si>
-  <si>
-    <t>R70</t>
-  </si>
-  <si>
-    <t>180K</t>
-  </si>
-  <si>
-    <t>RC0402FR-07180KL</t>
-  </si>
-  <si>
-    <t>R71</t>
-  </si>
-  <si>
-    <t>40K</t>
-  </si>
-  <si>
     <t>SCR0603F40K</t>
   </si>
   <si>
+    <t>SIM_I2C_SCL1</t>
+  </si>
+  <si>
+    <t>SIM_I2C_SCL</t>
+  </si>
+  <si>
+    <t>SIM_I2C_SDA1</t>
+  </si>
+  <si>
+    <t>SIM_I2C_SDA</t>
+  </si>
+  <si>
+    <t>SIM_PWR1, TP1, TP3, TP4</t>
+  </si>
+  <si>
+    <t>TestPoint</t>
+  </si>
+  <si>
     <t>SW1</t>
   </si>
   <si>
@@ -408,6 +537,36 @@
     <t>PRG18BC1R0MM1RB</t>
   </si>
   <si>
+    <t>TP2</t>
+  </si>
+  <si>
+    <t>BTN</t>
+  </si>
+  <si>
+    <t>TP5</t>
+  </si>
+  <si>
+    <t>BTN2</t>
+  </si>
+  <si>
+    <t>TP7</t>
+  </si>
+  <si>
+    <t>PA4</t>
+  </si>
+  <si>
+    <t>TP8</t>
+  </si>
+  <si>
+    <t>PB9</t>
+  </si>
+  <si>
+    <t>TP9</t>
+  </si>
+  <si>
+    <t>TestPoint:TestPoint_Pad_D1.5mm</t>
+  </si>
+  <si>
     <t>U1</t>
   </si>
   <si>
@@ -429,10 +588,13 @@
     <t>U3</t>
   </si>
   <si>
-    <t>SIM7000G</t>
-  </si>
-  <si>
-    <t>greencharge-footprints:SIM7000G</t>
+    <t>A9G_MODULE</t>
+  </si>
+  <si>
+    <t>MACHADA_footprints:A9G_MODULE</t>
+  </si>
+  <si>
+    <t>U4, U6, U10, U12, U18, U20</t>
   </si>
   <si>
     <t>TBU-CA065-200-WH</t>
@@ -441,12 +603,18 @@
     <t>MACHADA_footprints:TBU-CA065-200-WH</t>
   </si>
   <si>
+    <t>U5, U11, U19</t>
+  </si>
+  <si>
     <t>SSP3485U</t>
   </si>
   <si>
     <t>Package_SO:MSOP-8_3x3mm_P0.65mm</t>
   </si>
   <si>
+    <t>U7, U14</t>
+  </si>
+  <si>
     <t>WAS3157B</t>
   </si>
   <si>
@@ -462,6 +630,9 @@
     <t>Package_SO:SOIC-8_5.23x5.23mm_P1.27mm</t>
   </si>
   <si>
+    <t>U9, U13</t>
+  </si>
+  <si>
     <t>ATA6561-GAQW-N</t>
   </si>
   <si>
@@ -483,6 +654,24 @@
     <t>SY8089AAAC</t>
   </si>
   <si>
+    <t>Silergy</t>
+  </si>
+  <si>
+    <t>U17</t>
+  </si>
+  <si>
+    <t>XC6206PxxxMR</t>
+  </si>
+  <si>
+    <t>Package_TO_SOT_SMD:SOT-23-3</t>
+  </si>
+  <si>
+    <t>USB_VBUS1</t>
+  </si>
+  <si>
+    <t>USB_VBUS</t>
+  </si>
+  <si>
     <t>Y1</t>
   </si>
   <si>
@@ -492,6 +681,9 @@
     <t>Crystal:Crystal_SMD_3225-4Pin_3.2x2.5mm</t>
   </si>
   <si>
+    <t>Y2, Y3</t>
+  </si>
+  <si>
     <t>32.678KHz</t>
   </si>
   <si>
@@ -501,244 +693,7 @@
     <t>Q13FC1350000200</t>
   </si>
   <si>
-    <t>AE1, AE2</t>
-  </si>
-  <si>
-    <t>C1, C2, C3, C4, C5, C7, C8, C24, C25, C26, C30, C31, C33, C34, C39, C40, C41, C43, C44, C49, C50, C52</t>
-  </si>
-  <si>
-    <t>C6, C17, C21</t>
-  </si>
-  <si>
-    <t>C9, C10, C11, C12, C27, C28, C29</t>
-  </si>
-  <si>
-    <t>C13, C18, C19, C32, C42, C51</t>
-  </si>
-  <si>
-    <t>C15, C16</t>
-  </si>
-  <si>
-    <t>C46, C58</t>
-  </si>
-  <si>
-    <t>C56, C57</t>
-  </si>
-  <si>
-    <t>D7, D8, D13, D14, D16, D17</t>
-  </si>
-  <si>
-    <t>D9, D15, D18</t>
-  </si>
-  <si>
-    <t>D10, D11, D12</t>
-  </si>
-  <si>
-    <t>J1, J6</t>
-  </si>
-  <si>
-    <t>Q1, Q2</t>
-  </si>
-  <si>
-    <t>Q4, Q5</t>
-  </si>
-  <si>
-    <t>Q6, Q7, Q8, Q9, Q10, Q11</t>
-  </si>
-  <si>
-    <t>R2, R5, R6, R33, R34, R36, R40, R46, R47, R49, R50, R52, R53, R55, R56, R67, R69</t>
-  </si>
-  <si>
-    <t>R3, R4, R9, R31, R32, R58, R61, R65</t>
-  </si>
-  <si>
-    <t>R10, R12, R37, R39, R62, R64</t>
-  </si>
-  <si>
-    <t>R11, R15, R38, R63</t>
-  </si>
-  <si>
-    <t>R13, R14, R16</t>
-  </si>
-  <si>
-    <t>R17, R20</t>
-  </si>
-  <si>
-    <t>R19, R22, R29</t>
-  </si>
-  <si>
-    <t>R23, R24</t>
-  </si>
-  <si>
-    <t>R25, R26</t>
-  </si>
-  <si>
-    <t>R27, R28, R30</t>
-  </si>
-  <si>
-    <t>R35, R45, R48, R51, R54, R57</t>
-  </si>
-  <si>
-    <t>R43, R44, R59, R60</t>
-  </si>
-  <si>
-    <t>U4, U6, U10, U12, U18, U20</t>
-  </si>
-  <si>
-    <t>U5, U11, U19</t>
-  </si>
-  <si>
-    <t>U7, U14</t>
-  </si>
-  <si>
-    <t>U9, U13</t>
-  </si>
-  <si>
-    <t>Y2, Y3</t>
-  </si>
-  <si>
     <t>Vendor</t>
-  </si>
-  <si>
-    <t>2337019-1</t>
-  </si>
-  <si>
-    <t>BAT-HLD-012-SMT</t>
-  </si>
-  <si>
-    <t>CL05A104KA5NNNC</t>
-  </si>
-  <si>
-    <t>CL05A105KA5NQNC</t>
-  </si>
-  <si>
-    <t>CC0402JRNPO9BN220</t>
-  </si>
-  <si>
-    <t>CL05A106MP5NUNC</t>
-  </si>
-  <si>
-    <t>V0R3B0402C0G500NBT</t>
-  </si>
-  <si>
-    <t>CC0402KRX7R9BB103</t>
-  </si>
-  <si>
-    <t>CC0603JRNPO9BN330</t>
-  </si>
-  <si>
-    <t>CC0402KRX7R9BB102</t>
-  </si>
-  <si>
-    <t>0603B104K500NT</t>
-  </si>
-  <si>
-    <t>0603CG8R2C500NT</t>
-  </si>
-  <si>
-    <t>CC0603KRX7R9BB103</t>
-  </si>
-  <si>
-    <t>CC0603JRNPO9BN100</t>
-  </si>
-  <si>
-    <t>CL10A226MQ8NRNC</t>
-  </si>
-  <si>
-    <t>CL10A106MQ8NNNC</t>
-  </si>
-  <si>
-    <t>XL-1608SURC-06FJ</t>
-  </si>
-  <si>
-    <t>XL-1608UOC-06FJ</t>
-  </si>
-  <si>
-    <t>LTST-C191TBKT</t>
-  </si>
-  <si>
-    <t>SP0504BAHTG</t>
-  </si>
-  <si>
-    <t>BLM18BD421SH1D</t>
-  </si>
-  <si>
-    <t>SDFL1005Q1R0KTF</t>
-  </si>
-  <si>
-    <t>CBG160808U201T</t>
-  </si>
-  <si>
-    <t>LQG15HS27NJ02D</t>
-  </si>
-  <si>
-    <t>RC0402FR-0749R9L</t>
-  </si>
-  <si>
-    <t>RC0402FR-0710KL</t>
-  </si>
-  <si>
-    <t>RC0402FR-07100KL</t>
-  </si>
-  <si>
-    <t>RC0402FR-071ML</t>
-  </si>
-  <si>
-    <t>RC0402FR-07499RL</t>
-  </si>
-  <si>
-    <t>0402WGJ0100TCE</t>
-  </si>
-  <si>
-    <t>0402WGF2200TCE</t>
-  </si>
-  <si>
-    <t>RC0402JR-074K7L</t>
-  </si>
-  <si>
-    <t>RC0402FR-7W1KL</t>
-  </si>
-  <si>
-    <t>0402WGJ0000TCE</t>
-  </si>
-  <si>
-    <t>RC0603JR-072K2L</t>
-  </si>
-  <si>
-    <t>RC0402FR-07390RL</t>
-  </si>
-  <si>
-    <t>RC0402FR-0722RL</t>
-  </si>
-  <si>
-    <t>RC0402FR-0760R4L</t>
-  </si>
-  <si>
-    <t>RC0402JR-07100RL</t>
-  </si>
-  <si>
-    <t>SKRPACE010</t>
-  </si>
-  <si>
-    <t>STM32F103C8T6TR</t>
-  </si>
-  <si>
-    <t>PCF8523TK/1,118</t>
-  </si>
-  <si>
-    <t>WAS3157B-6/TR</t>
-  </si>
-  <si>
-    <t>W25Q32JVSSIQ</t>
-  </si>
-  <si>
-    <t>3225-8.00-18-10-10/4B</t>
-  </si>
-  <si>
-    <t>Digikey</t>
-  </si>
-  <si>
-    <t>LCSC</t>
   </si>
 </sst>
 </file>
@@ -881,7 +836,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1059,12 +1014,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1228,12 +1177,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1589,55 +1534,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F77"/>
+  <dimension ref="A1:F90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="D1" sqref="D1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" customWidth="1"/>
-    <col min="3" max="3" width="35" customWidth="1"/>
-    <col min="4" max="5" width="17.5546875" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="40.21875" customWidth="1"/>
+    <col min="4" max="5" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="E1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>158</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E2" t="s">
-        <v>236</v>
+        <v>7</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -1645,19 +1584,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>192</v>
-      </c>
-      <c r="E3" t="s">
-        <v>236</v>
+        <v>10</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1665,39 +1598,27 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>159</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E4" t="s">
-        <v>237</v>
+        <v>13</v>
       </c>
       <c r="F4">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>160</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="E5" t="s">
-        <v>237</v>
+        <v>13</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -1705,19 +1626,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>161</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="E6" t="s">
-        <v>237</v>
       </c>
       <c r="F6">
         <v>7</v>
@@ -1725,19 +1640,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>162</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E7" t="s">
-        <v>237</v>
+        <v>13</v>
       </c>
       <c r="F7">
         <v>6</v>
@@ -1745,59 +1654,44 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="E8" t="s">
-        <v>237</v>
+        <v>13</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>163</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="E9" t="s">
-        <v>237</v>
+        <v>13</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" t="s">
-        <v>237</v>
+        <v>26</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1805,39 +1699,27 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E11" t="s">
-        <v>237</v>
+        <v>28</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E12" t="s">
-        <v>237</v>
+        <v>13</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -1845,39 +1727,27 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>164</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" t="s">
-        <v>201</v>
-      </c>
-      <c r="E13" t="s">
-        <v>237</v>
+        <v>28</v>
       </c>
       <c r="F13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" t="s">
-        <v>202</v>
-      </c>
-      <c r="E14" t="s">
-        <v>237</v>
+        <v>28</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -1885,19 +1755,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
         <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" t="s">
-        <v>203</v>
-      </c>
-      <c r="E15" t="s">
-        <v>237</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -1905,19 +1769,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" t="s">
-        <v>199</v>
-      </c>
-      <c r="E16" t="s">
-        <v>237</v>
+        <v>28</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1925,39 +1783,27 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" t="s">
-        <v>204</v>
-      </c>
-      <c r="E17" t="s">
-        <v>237</v>
+        <v>28</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" t="s">
-        <v>205</v>
-      </c>
-      <c r="E18" t="s">
-        <v>237</v>
+        <v>42</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -1965,39 +1811,27 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>165</v>
+        <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" t="s">
-        <v>206</v>
-      </c>
-      <c r="E19" t="s">
-        <v>237</v>
+        <v>45</v>
       </c>
       <c r="F19">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" t="s">
-        <v>236</v>
+        <v>48</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -2005,19 +1839,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="E21" t="s">
-        <v>237</v>
+        <v>51</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -2025,19 +1853,13 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" t="s">
-        <v>237</v>
+        <v>45</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -2045,19 +1867,13 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
         <v>45</v>
-      </c>
-      <c r="C23" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="E23" t="s">
-        <v>237</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -2065,159 +1881,111 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="E24" t="s">
-        <v>237</v>
+        <v>42</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="E25" t="s">
-        <v>237</v>
+        <v>60</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>166</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C26" t="s">
-        <v>37</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E26" t="s">
-        <v>237</v>
+        <v>63</v>
       </c>
       <c r="F26">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>167</v>
+        <v>64</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
-      </c>
-      <c r="D27" t="s">
-        <v>52</v>
-      </c>
-      <c r="E27" t="s">
-        <v>237</v>
+        <v>66</v>
       </c>
       <c r="F27">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>168</v>
+        <v>67</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
-      </c>
-      <c r="D28" t="s">
-        <v>54</v>
-      </c>
-      <c r="E28" t="s">
-        <v>237</v>
+        <v>66</v>
       </c>
       <c r="F28">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="C29" t="s">
-        <v>58</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E29" t="s">
-        <v>236</v>
+        <v>71</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>169</v>
+        <v>72</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C30" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" s="1">
-        <v>1053142204</v>
-      </c>
-      <c r="E30" t="s">
-        <v>236</v>
+        <v>66</v>
       </c>
       <c r="F30">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="B31" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="C31" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" s="1">
-        <v>1053142206</v>
-      </c>
-      <c r="E31" t="s">
-        <v>236</v>
+        <v>66</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -2225,19 +1993,16 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B32" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="C32" t="s">
-        <v>63</v>
-      </c>
-      <c r="D32" s="1">
-        <v>1053142206</v>
-      </c>
-      <c r="E32" t="s">
-        <v>236</v>
+        <v>78</v>
+      </c>
+      <c r="D32">
+        <v>39301180</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -2245,19 +2010,16 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="C33" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="D33" t="s">
-        <v>69</v>
-      </c>
-      <c r="E33" t="s">
-        <v>236</v>
+        <v>82</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -2265,19 +2027,13 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="B34" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="C34" t="s">
-        <v>72</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="E34" t="s">
-        <v>237</v>
+        <v>85</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -2285,19 +2041,16 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="B35" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="C35" t="s">
-        <v>75</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="E35" t="s">
-        <v>237</v>
+        <v>88</v>
+      </c>
+      <c r="D35">
+        <v>5033981892</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -2305,19 +2058,13 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="C36" t="s">
-        <v>75</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="E36" t="s">
-        <v>237</v>
+        <v>91</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -2325,19 +2072,13 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="B37" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="C37" t="s">
-        <v>75</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="E37" t="s">
-        <v>237</v>
+        <v>91</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -2345,19 +2086,13 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="B38" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="C38" t="s">
-        <v>82</v>
-      </c>
-      <c r="D38" t="s">
-        <v>83</v>
-      </c>
-      <c r="E38" t="s">
-        <v>237</v>
+        <v>96</v>
       </c>
       <c r="F38">
         <v>1</v>
@@ -2365,39 +2100,30 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>170</v>
+        <v>97</v>
       </c>
       <c r="B39" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="C39" t="s">
-        <v>53</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E39" t="s">
-        <v>237</v>
+        <v>99</v>
       </c>
       <c r="F39">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="C40" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="D40" t="s">
-        <v>86</v>
-      </c>
-      <c r="E40" t="s">
-        <v>237</v>
+        <v>103</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -2405,19 +2131,13 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>171</v>
+        <v>104</v>
       </c>
       <c r="B41" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="C41" t="s">
-        <v>53</v>
-      </c>
-      <c r="D41" t="s">
-        <v>87</v>
-      </c>
-      <c r="E41" t="s">
-        <v>237</v>
+        <v>60</v>
       </c>
       <c r="F41">
         <v>2</v>
@@ -2425,299 +2145,209 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>172</v>
+        <v>106</v>
       </c>
       <c r="B42" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
       <c r="C42" t="s">
-        <v>53</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E42" t="s">
-        <v>237</v>
+        <v>60</v>
       </c>
       <c r="F42">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="B43" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="C43" t="s">
-        <v>91</v>
-      </c>
-      <c r="D43" t="s">
-        <v>215</v>
-      </c>
-      <c r="E43" t="s">
-        <v>237</v>
+        <v>60</v>
       </c>
       <c r="F43">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>173</v>
+        <v>110</v>
       </c>
       <c r="B44" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="C44" t="s">
-        <v>91</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="E44" t="s">
-        <v>237</v>
+        <v>60</v>
       </c>
       <c r="F44">
-        <v>17</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>174</v>
+        <v>112</v>
       </c>
       <c r="B45" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="C45" t="s">
-        <v>91</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="E45" t="s">
-        <v>237</v>
+        <v>114</v>
       </c>
       <c r="F45">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="B46" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="C46" t="s">
-        <v>91</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E46" t="s">
-        <v>237</v>
+        <v>114</v>
       </c>
       <c r="F46">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="B47" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="C47" t="s">
-        <v>91</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="E47" t="s">
-        <v>237</v>
+        <v>114</v>
       </c>
       <c r="F47">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>175</v>
+        <v>119</v>
       </c>
       <c r="B48" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="C48" t="s">
-        <v>91</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E48" t="s">
-        <v>237</v>
+        <v>114</v>
       </c>
       <c r="F48">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>176</v>
+        <v>121</v>
       </c>
       <c r="B49" t="s">
-        <v>99</v>
+        <v>122</v>
       </c>
       <c r="C49" t="s">
-        <v>91</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E49" t="s">
-        <v>237</v>
+        <v>114</v>
       </c>
       <c r="F49">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>177</v>
+        <v>123</v>
       </c>
       <c r="B50" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="C50" t="s">
-        <v>91</v>
-      </c>
-      <c r="D50" t="s">
-        <v>222</v>
-      </c>
-      <c r="E50" t="s">
-        <v>237</v>
+        <v>114</v>
       </c>
       <c r="F50">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>178</v>
+        <v>125</v>
       </c>
       <c r="B51" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="C51" t="s">
-        <v>91</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="E51" t="s">
-        <v>237</v>
+        <v>114</v>
       </c>
       <c r="F51">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="B52" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="C52" t="s">
-        <v>91</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E52" t="s">
-        <v>237</v>
+        <v>114</v>
       </c>
       <c r="F52">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>179</v>
+        <v>129</v>
       </c>
       <c r="B53" t="s">
-        <v>92</v>
+        <v>130</v>
       </c>
       <c r="C53" t="s">
-        <v>91</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="E53" t="s">
-        <v>237</v>
+        <v>114</v>
       </c>
       <c r="F53">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="B54" t="s">
-        <v>98</v>
+        <v>132</v>
       </c>
       <c r="C54" t="s">
-        <v>91</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E54" t="s">
-        <v>237</v>
+        <v>114</v>
       </c>
       <c r="F54">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>180</v>
+        <v>133</v>
       </c>
       <c r="B55" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="C55" t="s">
-        <v>106</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="E55" t="s">
-        <v>237</v>
+        <v>114</v>
       </c>
       <c r="F55">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>181</v>
+        <v>134</v>
       </c>
       <c r="B56" t="s">
-        <v>107</v>
+        <v>135</v>
       </c>
       <c r="C56" t="s">
-        <v>91</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E56" t="s">
-        <v>237</v>
+        <v>114</v>
       </c>
       <c r="F56">
         <v>2</v>
@@ -2725,19 +2355,13 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>182</v>
+        <v>136</v>
       </c>
       <c r="B57" t="s">
-        <v>108</v>
+        <v>137</v>
       </c>
       <c r="C57" t="s">
-        <v>91</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="E57" t="s">
-        <v>237</v>
+        <v>114</v>
       </c>
       <c r="F57">
         <v>3</v>
@@ -2745,119 +2369,83 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>183</v>
+        <v>138</v>
       </c>
       <c r="B58" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="C58" t="s">
-        <v>91</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="E58" t="s">
-        <v>237</v>
+        <v>114</v>
       </c>
       <c r="F58">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>184</v>
+        <v>140</v>
       </c>
       <c r="B59" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="C59" t="s">
-        <v>91</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="E59" t="s">
-        <v>237</v>
+        <v>114</v>
       </c>
       <c r="F59">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>111</v>
+        <v>141</v>
       </c>
       <c r="B60" t="s">
-        <v>101</v>
+        <v>142</v>
       </c>
       <c r="C60" t="s">
-        <v>91</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="E60" t="s">
-        <v>237</v>
+        <v>114</v>
       </c>
       <c r="F60">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="B61" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="C61" t="s">
-        <v>91</v>
-      </c>
-      <c r="D61" t="s">
-        <v>229</v>
-      </c>
-      <c r="E61" t="s">
-        <v>237</v>
+        <v>114</v>
       </c>
       <c r="F61">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>145</v>
+      </c>
+      <c r="B62" t="s">
+        <v>146</v>
+      </c>
+      <c r="C62" t="s">
         <v>114</v>
       </c>
-      <c r="B62" t="s">
-        <v>115</v>
-      </c>
-      <c r="C62" t="s">
-        <v>91</v>
-      </c>
-      <c r="D62" t="s">
-        <v>116</v>
-      </c>
-      <c r="E62" t="s">
-        <v>237</v>
-      </c>
       <c r="F62">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>117</v>
+        <v>147</v>
       </c>
       <c r="B63" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="C63" t="s">
-        <v>106</v>
-      </c>
-      <c r="D63" t="s">
-        <v>119</v>
-      </c>
-      <c r="E63" t="s">
-        <v>237</v>
+        <v>114</v>
       </c>
       <c r="F63">
         <v>1</v>
@@ -2865,19 +2453,13 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>120</v>
+        <v>148</v>
       </c>
       <c r="B64" t="s">
-        <v>121</v>
+        <v>149</v>
       </c>
       <c r="C64" t="s">
-        <v>122</v>
-      </c>
-      <c r="D64" t="s">
-        <v>230</v>
-      </c>
-      <c r="E64" t="s">
-        <v>237</v>
+        <v>114</v>
       </c>
       <c r="F64">
         <v>1</v>
@@ -2885,19 +2467,16 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>123</v>
+        <v>150</v>
       </c>
       <c r="B65" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="C65" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="D65" t="s">
-        <v>126</v>
-      </c>
-      <c r="E65" t="s">
-        <v>236</v>
+        <v>152</v>
       </c>
       <c r="F65">
         <v>1</v>
@@ -2905,19 +2484,16 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="B66" t="s">
-        <v>128</v>
+        <v>154</v>
       </c>
       <c r="C66" t="s">
-        <v>129</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="E66" t="s">
-        <v>237</v>
+        <v>155</v>
+      </c>
+      <c r="D66" t="s">
+        <v>156</v>
       </c>
       <c r="F66">
         <v>1</v>
@@ -2925,19 +2501,13 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>130</v>
+        <v>157</v>
       </c>
       <c r="B67" t="s">
-        <v>131</v>
+        <v>158</v>
       </c>
       <c r="C67" t="s">
-        <v>132</v>
-      </c>
-      <c r="D67" t="s">
-        <v>232</v>
-      </c>
-      <c r="E67" t="s">
-        <v>236</v>
+        <v>66</v>
       </c>
       <c r="F67">
         <v>1</v>
@@ -2945,19 +2515,13 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>133</v>
+        <v>159</v>
       </c>
       <c r="B68" t="s">
-        <v>134</v>
+        <v>160</v>
       </c>
       <c r="C68" t="s">
-        <v>135</v>
-      </c>
-      <c r="D68" t="s">
-        <v>134</v>
-      </c>
-      <c r="E68" t="s">
-        <v>236</v>
+        <v>66</v>
       </c>
       <c r="F68">
         <v>1</v>
@@ -2965,79 +2529,58 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
       <c r="B69" t="s">
-        <v>136</v>
+        <v>162</v>
       </c>
       <c r="C69" t="s">
-        <v>137</v>
-      </c>
-      <c r="D69" t="s">
-        <v>136</v>
-      </c>
-      <c r="E69" t="s">
-        <v>237</v>
+        <v>66</v>
       </c>
       <c r="F69">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>186</v>
+        <v>163</v>
       </c>
       <c r="B70" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="C70" t="s">
-        <v>139</v>
-      </c>
-      <c r="D70" t="s">
-        <v>138</v>
-      </c>
-      <c r="E70" t="s">
-        <v>237</v>
+        <v>165</v>
       </c>
       <c r="F70">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="B71" t="s">
-        <v>140</v>
+        <v>167</v>
       </c>
       <c r="C71" t="s">
-        <v>141</v>
+        <v>168</v>
       </c>
       <c r="D71" t="s">
-        <v>233</v>
-      </c>
-      <c r="E71" t="s">
-        <v>237</v>
+        <v>169</v>
       </c>
       <c r="F71">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>142</v>
+        <v>170</v>
       </c>
       <c r="B72" t="s">
-        <v>143</v>
+        <v>171</v>
       </c>
       <c r="C72" t="s">
-        <v>144</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="E72" t="s">
-        <v>237</v>
+        <v>66</v>
       </c>
       <c r="F72">
         <v>1</v>
@@ -3045,39 +2588,27 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="B73" t="s">
-        <v>145</v>
+        <v>173</v>
       </c>
       <c r="C73" t="s">
-        <v>146</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E73" t="s">
-        <v>237</v>
+        <v>66</v>
       </c>
       <c r="F73">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="B74" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="C74" t="s">
-        <v>149</v>
-      </c>
-      <c r="D74" t="s">
-        <v>148</v>
-      </c>
-      <c r="E74" t="s">
-        <v>237</v>
+        <v>66</v>
       </c>
       <c r="F74">
         <v>1</v>
@@ -3085,19 +2616,13 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>150</v>
+        <v>176</v>
       </c>
       <c r="B75" t="s">
-        <v>151</v>
+        <v>177</v>
       </c>
       <c r="C75" t="s">
-        <v>50</v>
-      </c>
-      <c r="D75" t="s">
-        <v>151</v>
-      </c>
-      <c r="E75" t="s">
-        <v>237</v>
+        <v>66</v>
       </c>
       <c r="F75">
         <v>1</v>
@@ -3105,19 +2630,13 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>152</v>
+        <v>178</v>
       </c>
       <c r="B76" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="C76" t="s">
-        <v>154</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="E76" t="s">
-        <v>237</v>
+        <v>179</v>
       </c>
       <c r="F76">
         <v>1</v>
@@ -3125,21 +2644,203 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
+        <v>180</v>
+      </c>
+      <c r="B77" t="s">
+        <v>181</v>
+      </c>
+      <c r="C77" t="s">
+        <v>182</v>
+      </c>
+      <c r="F77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>183</v>
+      </c>
+      <c r="B78" t="s">
+        <v>184</v>
+      </c>
+      <c r="C78" t="s">
+        <v>185</v>
+      </c>
+      <c r="F78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>186</v>
+      </c>
+      <c r="B79" t="s">
+        <v>187</v>
+      </c>
+      <c r="C79" t="s">
+        <v>188</v>
+      </c>
+      <c r="F79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>189</v>
       </c>
-      <c r="B77" t="s">
-        <v>155</v>
-      </c>
-      <c r="C77" t="s">
-        <v>156</v>
-      </c>
-      <c r="D77" t="s">
-        <v>157</v>
-      </c>
-      <c r="E77" t="s">
-        <v>237</v>
-      </c>
-      <c r="F77">
+      <c r="B80" t="s">
+        <v>190</v>
+      </c>
+      <c r="C80" t="s">
+        <v>191</v>
+      </c>
+      <c r="F80">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>192</v>
+      </c>
+      <c r="B81" t="s">
+        <v>193</v>
+      </c>
+      <c r="C81" t="s">
+        <v>194</v>
+      </c>
+      <c r="F81">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>195</v>
+      </c>
+      <c r="B82" t="s">
+        <v>196</v>
+      </c>
+      <c r="C82" t="s">
+        <v>197</v>
+      </c>
+      <c r="F82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>198</v>
+      </c>
+      <c r="B83" t="s">
+        <v>199</v>
+      </c>
+      <c r="C83" t="s">
+        <v>200</v>
+      </c>
+      <c r="F83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>201</v>
+      </c>
+      <c r="B84" t="s">
+        <v>202</v>
+      </c>
+      <c r="C84" t="s">
+        <v>203</v>
+      </c>
+      <c r="F84">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>204</v>
+      </c>
+      <c r="B85" t="s">
+        <v>205</v>
+      </c>
+      <c r="C85" t="s">
+        <v>206</v>
+      </c>
+      <c r="F85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>207</v>
+      </c>
+      <c r="B86" t="s">
+        <v>208</v>
+      </c>
+      <c r="C86" t="s">
+        <v>51</v>
+      </c>
+      <c r="E86" t="s">
+        <v>209</v>
+      </c>
+      <c r="F86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>210</v>
+      </c>
+      <c r="B87" t="s">
+        <v>211</v>
+      </c>
+      <c r="C87" t="s">
+        <v>212</v>
+      </c>
+      <c r="F87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>213</v>
+      </c>
+      <c r="B88" t="s">
+        <v>214</v>
+      </c>
+      <c r="C88" t="s">
+        <v>66</v>
+      </c>
+      <c r="F88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>215</v>
+      </c>
+      <c r="B89" t="s">
+        <v>216</v>
+      </c>
+      <c r="C89" t="s">
+        <v>217</v>
+      </c>
+      <c r="F89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>218</v>
+      </c>
+      <c r="B90" t="s">
+        <v>219</v>
+      </c>
+      <c r="C90" t="s">
+        <v>220</v>
+      </c>
+      <c r="D90" t="s">
+        <v>221</v>
+      </c>
+      <c r="F90">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
completed project and all the prouction files
</commit_message>
<xml_diff>
--- a/BOM/BIM_PCB.xlsx
+++ b/BOM/BIM_PCB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\kicad6\KICAD 6.0.0\contractual_projects\ECO_BODA\BIM_PCB\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F53CFDF-020D-46D5-BA82-FB9AEAA6C7DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{F568B3CA-6C2F-4E63-9535-DD0F53A53C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="BIM_PCB" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="365" uniqueCount="231">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="370" uniqueCount="233">
   <si>
     <t>Qty</t>
   </si>
@@ -42,12 +42,21 @@
     <t>MPN</t>
   </si>
   <si>
-    <t>AE1, AE2</t>
+    <t>AE1</t>
   </si>
   <si>
     <t>Antenna_Shield</t>
   </si>
   <si>
+    <t>Connector_Coaxial:SMA_Samtec_SMA-J-P-X-ST-EM1_EdgeMount</t>
+  </si>
+  <si>
+    <t>SMA-KE-347-H13.5-1.2</t>
+  </si>
+  <si>
+    <t>AE2, AE3</t>
+  </si>
+  <si>
     <t>greencharge-footprints:UFL_COAX_CONN23370191</t>
   </si>
   <si>
@@ -60,7 +69,7 @@
     <t>Battery:BatteryHolder_LINX_BAT-HLD-012-SMT</t>
   </si>
   <si>
-    <t>C1, C2, C3, C4, C5, C7, C8, C24, C25, C30, C31, C33, C34, C39, C40, C41, C43, C44, C49, C50, C52</t>
+    <t>C1, C2, C3, C4, C5, C7, C8, C24, C25, C30, C31, C33, C34, C39, C40, C41, C43, C44, C46, C49, C50, C52, C58</t>
   </si>
   <si>
     <t>100n</t>
@@ -87,7 +96,7 @@
     <t>10u</t>
   </si>
   <si>
-    <t>C14, C16, C21</t>
+    <t>C14, C16, C21, C28</t>
   </si>
   <si>
     <t>0.1u</t>
@@ -96,7 +105,7 @@
     <t>C15, C17, C22</t>
   </si>
   <si>
-    <t>C28</t>
+    <t>C35, C36</t>
   </si>
   <si>
     <t>100u</t>
@@ -108,24 +117,21 @@
     <t>TLJA107M006R0800</t>
   </si>
   <si>
-    <t>C46, C58</t>
+    <t>C47</t>
+  </si>
+  <si>
+    <t>8.2p</t>
+  </si>
+  <si>
+    <t>C48</t>
+  </si>
+  <si>
+    <t>10n</t>
   </si>
   <si>
     <t>Capacitor_SMD:C_0603_1608Metric</t>
   </si>
   <si>
-    <t>C47</t>
-  </si>
-  <si>
-    <t>8.2p</t>
-  </si>
-  <si>
-    <t>C48</t>
-  </si>
-  <si>
-    <t>10n</t>
-  </si>
-  <si>
     <t>C53</t>
   </si>
   <si>
@@ -189,6 +195,9 @@
     <t>ORANGE</t>
   </si>
   <si>
+    <t>LED_SMD:LED_0402_1005Metric</t>
+  </si>
+  <si>
     <t>D6</t>
   </si>
   <si>
@@ -210,13 +219,28 @@
     <t>Package_TO_SOT_SMD:SOT-23</t>
   </si>
   <si>
-    <t>D10, D11, D12</t>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>RS1K-E3/5ATSS310</t>
+  </si>
+  <si>
+    <t>Diode_SMD:D_SMA</t>
+  </si>
+  <si>
+    <t>D11, D12</t>
   </si>
   <si>
     <t>SS310</t>
   </si>
   <si>
-    <t>Diode_SMD:D_SMA</t>
+    <t>FL1</t>
+  </si>
+  <si>
+    <t>SAFEB1G57KE0F00R15</t>
+  </si>
+  <si>
+    <t>Filter:Filter_1411-5_1.4x1.1mm</t>
   </si>
   <si>
     <t>J1</t>
@@ -225,6 +249,12 @@
     <t>Conn_02x09_Counter_Clockwise</t>
   </si>
   <si>
+    <t>MACHADA_footprints:conn_18pin_02x09_angled_MX23A18NF1</t>
+  </si>
+  <si>
+    <t>MX23A18NF1</t>
+  </si>
+  <si>
     <t>J2</t>
   </si>
   <si>
@@ -234,9 +264,6 @@
     <t>MACHADA_footprints:nano_sim_NSIM-2-C</t>
   </si>
   <si>
-    <t>NSIM-2-C</t>
-  </si>
-  <si>
     <t>J4</t>
   </si>
   <si>
@@ -288,18 +315,9 @@
     <t>IRLML0100TRPBF</t>
   </si>
   <si>
-    <t>Q4, Q7, Q8, Q9</t>
-  </si>
-  <si>
-    <t>2N7002</t>
-  </si>
-  <si>
     <t>Q5, Q6</t>
   </si>
   <si>
-    <t>BSN20</t>
-  </si>
-  <si>
     <t>R1</t>
   </si>
   <si>
@@ -309,7 +327,7 @@
     <t>Resistor_SMD:R_0402_1005Metric</t>
   </si>
   <si>
-    <t>R2, R5, R6, R17, R18, R48, R49, R51, R52, R54, R55, R67, R69</t>
+    <t>R2, R5, R6, R67, R69</t>
   </si>
   <si>
     <t>10K</t>
@@ -351,12 +369,6 @@
     <t>4.7K</t>
   </si>
   <si>
-    <t>R19, R50, R53, R56</t>
-  </si>
-  <si>
-    <t>1K</t>
-  </si>
-  <si>
     <t>R20, R23, R24</t>
   </si>
   <si>
@@ -405,6 +417,12 @@
     <t>60R</t>
   </si>
   <si>
+    <t>R51</t>
+  </si>
+  <si>
+    <t>0R</t>
+  </si>
+  <si>
     <t>R66</t>
   </si>
   <si>
@@ -582,9 +600,6 @@
     <t>BAT-HLD-012-SMT</t>
   </si>
   <si>
-    <t>Digikey</t>
-  </si>
-  <si>
     <t>CL05A104KA5NNNC</t>
   </si>
   <si>
@@ -597,7 +612,7 @@
     <t>CL05A106MP5NUNC</t>
   </si>
   <si>
-    <t>0603B104K500NT</t>
+    <t>CL05C8R2CB51PNC</t>
   </si>
   <si>
     <t>CC0603KRX7R9BB103</t>
@@ -615,116 +630,107 @@
     <t>CL10A106MQ8NNNC</t>
   </si>
   <si>
-    <t>CL05C8R2CB51PNC</t>
-  </si>
-  <si>
     <t>XL-1608SURC-06FJ</t>
   </si>
   <si>
+    <t>XL-1608UOC-06FJ</t>
+  </si>
+  <si>
+    <t>LTST-C191TBKT</t>
+  </si>
+  <si>
+    <t>SP0504BAHTG</t>
+  </si>
+  <si>
+    <t>ZX-NSIM-281.4J</t>
+  </si>
+  <si>
+    <t>BLM18BD421SH1D</t>
+  </si>
+  <si>
+    <t>SDCL1005C82NJTDF</t>
+  </si>
+  <si>
+    <t>RC0402FR-0749R9L</t>
+  </si>
+  <si>
+    <t>RC0402FR-0710KL</t>
+  </si>
+  <si>
+    <t>RC0402FR-07100KL</t>
+  </si>
+  <si>
+    <t>RC0402FR-071ML</t>
+  </si>
+  <si>
+    <t>RC0402FR-07499RL</t>
+  </si>
+  <si>
+    <t>0402WGJ0100TCE</t>
+  </si>
+  <si>
+    <t>0402WGF2200TCE</t>
+  </si>
+  <si>
+    <t>RC0402JR-074K7L</t>
+  </si>
+  <si>
+    <t>RC0402FR-7W1KL</t>
+  </si>
+  <si>
+    <t>RC0402FR-072K2L</t>
+  </si>
+  <si>
+    <t>RC0402FR-0722RL</t>
+  </si>
+  <si>
+    <t>RC0402FR-07200KL</t>
+  </si>
+  <si>
+    <t>RC0402FR-07390RL</t>
+  </si>
+  <si>
+    <t>RC0402FR-0760R4L</t>
+  </si>
+  <si>
+    <t>0402WGJ0000TCE</t>
+  </si>
+  <si>
+    <t>RC0402JR-07100RL</t>
+  </si>
+  <si>
+    <t>SKRPACE010</t>
+  </si>
+  <si>
+    <t>STM32F103C8T6TR</t>
+  </si>
+  <si>
+    <t>PCF8523TK/1,118</t>
+  </si>
+  <si>
+    <t>A9G</t>
+  </si>
+  <si>
+    <t>WAS3157B-6/TR</t>
+  </si>
+  <si>
+    <t>W25Q32JVSSIQ</t>
+  </si>
+  <si>
+    <t>XC6206P282MR</t>
+  </si>
+  <si>
+    <t>3225-8.00-18-10-10/4B</t>
+  </si>
+  <si>
     <t>LCSC</t>
-  </si>
-  <si>
-    <t>XL-1608UOC-06FJ</t>
-  </si>
-  <si>
-    <t>LTST-C191TBKT</t>
-  </si>
-  <si>
-    <t>SP0504BAHTG</t>
-  </si>
-  <si>
-    <t>BLM18BD421SH1D</t>
-  </si>
-  <si>
-    <t>RC0402FR-0749R9L</t>
-  </si>
-  <si>
-    <t>RC0402FR-0710KL</t>
-  </si>
-  <si>
-    <t>RC0402FR-07100KL</t>
-  </si>
-  <si>
-    <t>RC0402FR-071ML</t>
-  </si>
-  <si>
-    <t>RC0402FR-07499RL</t>
-  </si>
-  <si>
-    <t>0402WGJ0100TCE</t>
-  </si>
-  <si>
-    <t>0402WGF2200TCE</t>
-  </si>
-  <si>
-    <t>RC0402JR-074K7L</t>
-  </si>
-  <si>
-    <t>RC0402FR-7W1KL</t>
-  </si>
-  <si>
-    <t>RC0402FR-0722RL</t>
-  </si>
-  <si>
-    <t>RC0402FR-07390RL</t>
-  </si>
-  <si>
-    <t>RC0402FR-0760R4L</t>
-  </si>
-  <si>
-    <t>RC0402JR-07100RL</t>
-  </si>
-  <si>
-    <t>SKRPACE010</t>
-  </si>
-  <si>
-    <t>STM32F103C8T6TR</t>
-  </si>
-  <si>
-    <t>PCF8523TK/1,118</t>
-  </si>
-  <si>
-    <t>WAS3157B-6/TR</t>
-  </si>
-  <si>
-    <t>W25Q32JVSSIQ</t>
-  </si>
-  <si>
-    <t>3225-8.00-18-10-10/4B</t>
-  </si>
-  <si>
-    <t>A9G</t>
-  </si>
-  <si>
-    <t>XC6206P282MR</t>
-  </si>
-  <si>
-    <t>1k/0K</t>
-  </si>
-  <si>
-    <t>RC0402FR-07200KL</t>
-  </si>
-  <si>
-    <t>RC0402FR-072K2L</t>
-  </si>
-  <si>
-    <t>MACHADA_footprints:conn_18pin_02x09_angled_MX23A18NF1</t>
-  </si>
-  <si>
-    <t>MX23A18NF1</t>
-  </si>
-  <si>
-    <t>SDCL1005C82NJTDF</t>
-  </si>
-  <si>
-    <t>RC0402FR-071KL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -859,6 +865,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -1042,7 +1056,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1163,7 +1177,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1206,16 +1220,17 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1249,6 +1264,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1568,39 +1584,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F73"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" customWidth="1"/>
-    <col min="3" max="3" width="40.33203125" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" customWidth="1"/>
+    <col min="3" max="3" width="51" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1614,34 +1629,34 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>183</v>
+      <c r="D2" t="s">
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>185</v>
+        <v>232</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>184</v>
+      <c r="D3" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="E3" t="s">
-        <v>185</v>
+        <v>232</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1654,14 +1669,14 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>186</v>
+      <c r="D4" t="s">
+        <v>190</v>
       </c>
       <c r="E4" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F4">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1672,133 +1687,133 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="E5" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="E6" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F6">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="E7" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F7">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>186</v>
+        <v>16</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="E8" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F8">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>187</v>
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>191</v>
       </c>
       <c r="E9" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F9">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>26</v>
+        <v>16</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="E10" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
         <v>27</v>
-      </c>
-      <c r="B11" t="s">
-        <v>12</v>
       </c>
       <c r="C11" t="s">
         <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>190</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F11">
         <v>2</v>
@@ -1806,19 +1821,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E12" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -1826,19 +1841,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="E13" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -1846,19 +1861,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
         <v>34</v>
       </c>
-      <c r="C14" t="s">
-        <v>28</v>
-      </c>
       <c r="D14" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="E14" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -1866,19 +1881,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="E15" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -1886,19 +1901,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="E16" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1906,19 +1921,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="E17" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F17">
         <v>2</v>
@@ -1926,19 +1941,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E18" t="s">
-        <v>185</v>
+        <v>232</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -1946,19 +1961,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="E19" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -1966,19 +1981,19 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -1986,19 +2001,19 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E21" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -2006,19 +2021,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="E22" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -2026,19 +2041,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="E23" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -2046,19 +2061,19 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E24" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F24">
         <v>6</v>
@@ -2066,19 +2081,19 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C25" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D25" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E25" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F25">
         <v>3</v>
@@ -2086,59 +2101,59 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D26" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E26" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F26">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B27" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C27" t="s">
-        <v>227</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>228</v>
+        <v>66</v>
+      </c>
+      <c r="D27" t="s">
+        <v>68</v>
       </c>
       <c r="E27" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F27">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B28" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C28" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D28" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E28" t="s">
-        <v>185</v>
+        <v>232</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -2146,19 +2161,19 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
-      </c>
-      <c r="D29">
-        <v>5033981892</v>
+        <v>74</v>
+      </c>
+      <c r="D29" t="s">
+        <v>75</v>
       </c>
       <c r="E29" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -2166,59 +2181,59 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B30" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C30" t="s">
-        <v>75</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>202</v>
+        <v>78</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>205</v>
       </c>
       <c r="E30" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F30">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="F31" s="3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31">
+        <v>5033981892</v>
+      </c>
+      <c r="E31" t="s">
+        <v>232</v>
+      </c>
+      <c r="F31">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B32" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C32" t="s">
-        <v>81</v>
-      </c>
-      <c r="D32" t="s">
-        <v>82</v>
+        <v>84</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>206</v>
       </c>
       <c r="E32" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -2226,39 +2241,39 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B33" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C33" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
+      </c>
+      <c r="D33" t="s">
+        <v>207</v>
       </c>
       <c r="E33" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F33">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B34" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C34" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="D34" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="E34" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -2266,139 +2281,139 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B35" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C35" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E35" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F35">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B36" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C36" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D36" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="E36" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F36">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B37" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C37" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="D37" t="s">
-        <v>203</v>
+        <v>95</v>
       </c>
       <c r="E37" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F37">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B38" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C38" t="s">
-        <v>93</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>204</v>
+        <v>99</v>
+      </c>
+      <c r="D38" t="s">
+        <v>208</v>
       </c>
       <c r="E38" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F38">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B39" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C39" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="E39" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F39">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B40" t="s">
+        <v>103</v>
+      </c>
+      <c r="C40" t="s">
         <v>99</v>
       </c>
-      <c r="C40" t="s">
-        <v>93</v>
-      </c>
       <c r="D40" s="1" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="E40" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B41" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C41" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="E41" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F41">
         <v>1</v>
@@ -2406,119 +2421,119 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B42" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C42" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="E42" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F42">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B43" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C43" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="E43" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F43">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B44" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C44" t="s">
-        <v>93</v>
-      </c>
-      <c r="D44" t="s">
-        <v>210</v>
+        <v>99</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>214</v>
       </c>
       <c r="E44" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F44">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B45" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C45" t="s">
-        <v>93</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>211</v>
+        <v>99</v>
+      </c>
+      <c r="D45" t="s">
+        <v>215</v>
       </c>
       <c r="E45" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F45">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="F46" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>114</v>
+      </c>
+      <c r="B46" t="s">
+        <v>115</v>
+      </c>
+      <c r="C46" t="s">
+        <v>99</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E46" t="s">
+        <v>232</v>
+      </c>
+      <c r="F46">
         <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B47" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="C47" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="E47" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F47">
         <v>3</v>
@@ -2526,19 +2541,19 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B48" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C48" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D48" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="E48" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F48">
         <v>2</v>
@@ -2546,19 +2561,19 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B49" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C49" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="E49" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F49">
         <v>3</v>
@@ -2566,19 +2581,19 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B50" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C50" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D50" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="E50" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F50">
         <v>1</v>
@@ -2586,19 +2601,19 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B51" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="C51" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="E51" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F51">
         <v>1</v>
@@ -2606,19 +2621,19 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B52" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C52" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="E52" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F52">
         <v>2</v>
@@ -2626,19 +2641,19 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B53" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C53" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="E53" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F53">
         <v>6</v>
@@ -2646,19 +2661,19 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B54" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C54" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="E54" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F54">
         <v>4</v>
@@ -2666,19 +2681,19 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B55" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
       <c r="C55" t="s">
-        <v>93</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>211</v>
+        <v>99</v>
+      </c>
+      <c r="D55" t="s">
+        <v>222</v>
       </c>
       <c r="E55" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F55">
         <v>1</v>
@@ -2686,19 +2701,19 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B56" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="C56" t="s">
-        <v>93</v>
-      </c>
-      <c r="D56" t="s">
-        <v>215</v>
+        <v>99</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="E56" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F56">
         <v>1</v>
@@ -2706,19 +2721,19 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B57" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C57" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D57" t="s">
-        <v>131</v>
+        <v>223</v>
       </c>
       <c r="E57" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F57">
         <v>1</v>
@@ -2726,19 +2741,19 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B58" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C58" t="s">
-        <v>134</v>
+        <v>99</v>
       </c>
       <c r="D58" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E58" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F58">
         <v>1</v>
@@ -2746,19 +2761,19 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B59" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C59" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D59" t="s">
-        <v>216</v>
+        <v>141</v>
       </c>
       <c r="E59" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F59">
         <v>1</v>
@@ -2766,19 +2781,19 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B60" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C60" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D60" t="s">
-        <v>142</v>
+        <v>224</v>
       </c>
       <c r="E60" t="s">
-        <v>185</v>
+        <v>232</v>
       </c>
       <c r="F60">
         <v>1</v>
@@ -2786,19 +2801,19 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B61" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C61" t="s">
-        <v>145</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>217</v>
+        <v>147</v>
+      </c>
+      <c r="D61" t="s">
+        <v>148</v>
       </c>
       <c r="E61" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F61">
         <v>1</v>
@@ -2806,19 +2821,19 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B62" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C62" t="s">
-        <v>148</v>
-      </c>
-      <c r="D62" t="s">
-        <v>218</v>
+        <v>151</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>225</v>
       </c>
       <c r="E62" t="s">
-        <v>185</v>
+        <v>232</v>
       </c>
       <c r="F62">
         <v>1</v>
@@ -2826,19 +2841,19 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B63" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C63" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="D63" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="E63" t="s">
-        <v>185</v>
+        <v>232</v>
       </c>
       <c r="F63">
         <v>1</v>
@@ -2846,139 +2861,139 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B64" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C64" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="D64" t="s">
-        <v>153</v>
+        <v>227</v>
       </c>
       <c r="E64" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F64">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B65" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C65" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D65" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="E65" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F65">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B66" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C66" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="D66" t="s">
-        <v>219</v>
+        <v>162</v>
       </c>
       <c r="E66" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F66">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B67" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C67" t="s">
-        <v>163</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>220</v>
+        <v>166</v>
+      </c>
+      <c r="D67" t="s">
+        <v>228</v>
       </c>
       <c r="E67" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F67">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B68" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C68" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>165</v>
+        <v>229</v>
       </c>
       <c r="E68" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F68">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B69" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C69" t="s">
-        <v>169</v>
-      </c>
-      <c r="D69" t="s">
-        <v>168</v>
+        <v>172</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>171</v>
       </c>
       <c r="E69" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F69">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B70" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C70" t="s">
-        <v>51</v>
+        <v>175</v>
       </c>
       <c r="D70" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E70" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F70">
         <v>1</v>
@@ -2986,19 +3001,19 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="B71" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="C71" t="s">
-        <v>174</v>
+        <v>53</v>
       </c>
       <c r="D71" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="E71" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F71">
         <v>1</v>
@@ -3006,19 +3021,19 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B72" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C72" t="s">
-        <v>177</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>221</v>
+        <v>180</v>
+      </c>
+      <c r="D72" t="s">
+        <v>230</v>
       </c>
       <c r="E72" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F72">
         <v>1</v>
@@ -3026,26 +3041,49 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B73" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C73" t="s">
-        <v>180</v>
-      </c>
-      <c r="D73" t="s">
-        <v>181</v>
+        <v>183</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>231</v>
       </c>
       <c r="E73" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
       <c r="F73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>184</v>
+      </c>
+      <c r="B74" t="s">
+        <v>185</v>
+      </c>
+      <c r="C74" t="s">
+        <v>186</v>
+      </c>
+      <c r="D74" t="s">
+        <v>187</v>
+      </c>
+      <c r="E74" t="s">
+        <v>232</v>
+      </c>
+      <c r="F74">
         <v>2</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D30" r:id="rId1" display="https://www.lcsc.com/product-detail/span-style-background-color-ff0-SIM-span-Card-Connectors_Megastar-ZX-NSIM-281-4J_C7419853.html"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
BIM updated BOM and placement files guide pdf added
</commit_message>
<xml_diff>
--- a/BOM/BIM_PCB.xlsx
+++ b/BOM/BIM_PCB.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\kicad6\KICAD 6.0.0\contractual_projects\ECO_BODA\BIM_PCB\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{F568B3CA-6C2F-4E63-9535-DD0F53A53C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD7DDDB4-25F9-49E4-ADD6-028E58386E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="370" uniqueCount="233">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="379" uniqueCount="233">
   <si>
     <t>Qty</t>
   </si>
@@ -42,19 +42,22 @@
     <t>MPN</t>
   </si>
   <si>
+    <t>Manufacturer_Name</t>
+  </si>
+  <si>
     <t>AE1</t>
   </si>
   <si>
     <t>Antenna_Shield</t>
   </si>
   <si>
-    <t>Connector_Coaxial:SMA_Samtec_SMA-J-P-X-ST-EM1_EdgeMount</t>
-  </si>
-  <si>
-    <t>SMA-KE-347-H13.5-1.2</t>
-  </si>
-  <si>
-    <t>AE2, AE3</t>
+    <t>Connector_Coaxial:SMA_Molex_73251-2200_Horizontal</t>
+  </si>
+  <si>
+    <t>BWSMA-KWE-Z001</t>
+  </si>
+  <si>
+    <t>AE2</t>
   </si>
   <si>
     <t>greencharge-footprints:UFL_COAX_CONN23370191</t>
@@ -96,13 +99,19 @@
     <t>10u</t>
   </si>
   <si>
-    <t>C14, C16, C21, C28</t>
+    <t>C14, C16, C28, C37</t>
   </si>
   <si>
     <t>0.1u</t>
   </si>
   <si>
-    <t>C15, C17, C22</t>
+    <t>C15, C17, C38</t>
+  </si>
+  <si>
+    <t>C21, C22</t>
+  </si>
+  <si>
+    <t>C_Small</t>
   </si>
   <si>
     <t>C35, C36</t>
@@ -168,7 +177,7 @@
     <t>LED</t>
   </si>
   <si>
-    <t>LED_SMD:LED_0603_1608Metric</t>
+    <t>LED_SMD:LED_0402_1005Metric</t>
   </si>
   <si>
     <t>D3</t>
@@ -195,9 +204,6 @@
     <t>ORANGE</t>
   </si>
   <si>
-    <t>LED_SMD:LED_0402_1005Metric</t>
-  </si>
-  <si>
     <t>D6</t>
   </si>
   <si>
@@ -219,7 +225,7 @@
     <t>Package_TO_SOT_SMD:SOT-23</t>
   </si>
   <si>
-    <t>D10</t>
+    <t>D10, D11, D12</t>
   </si>
   <si>
     <t>RS1K-E3/5ATSS310</t>
@@ -228,10 +234,10 @@
     <t>Diode_SMD:D_SMA</t>
   </si>
   <si>
-    <t>D11, D12</t>
-  </si>
-  <si>
-    <t>SS310</t>
+    <t>D19</t>
+  </si>
+  <si>
+    <t>4.4-4.5 ZENER</t>
   </si>
   <si>
     <t>FL1</t>
@@ -264,7 +270,10 @@
     <t>MACHADA_footprints:nano_sim_NSIM-2-C</t>
   </si>
   <si>
-    <t>J4</t>
+    <t>NSIM-2-C</t>
+  </si>
+  <si>
+    <t>J7</t>
   </si>
   <si>
     <t>Micro_SD_Card</t>
@@ -279,7 +288,7 @@
     <t>L_Ferrite</t>
   </si>
   <si>
-    <t>Inductor_SMD:L_0603_1608Metric</t>
+    <t>Inductor_SMD:L_0402_1005Metric</t>
   </si>
   <si>
     <t>L2</t>
@@ -288,7 +297,10 @@
     <t>82nH</t>
   </si>
   <si>
-    <t>Inductor_SMD:L_0402_1005Metric</t>
+    <t>L3, L4, L6, L7, L8, L9</t>
+  </si>
+  <si>
+    <t>ferrite bead</t>
   </si>
   <si>
     <t>L5</t>
@@ -318,7 +330,7 @@
     <t>Q5, Q6</t>
   </si>
   <si>
-    <t>R1</t>
+    <t>R1, R18</t>
   </si>
   <si>
     <t>49.9R</t>
@@ -369,6 +381,18 @@
     <t>4.7K</t>
   </si>
   <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>22R</t>
+  </si>
+  <si>
+    <t>R19, R40, R41, R42, R45, R46</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
     <t>R20, R23, R24</t>
   </si>
   <si>
@@ -387,9 +411,6 @@
     <t>R28, R29, R30</t>
   </si>
   <si>
-    <t>22R</t>
-  </si>
-  <si>
     <t>R33</t>
   </si>
   <si>
@@ -405,12 +426,6 @@
     <t>390R</t>
   </si>
   <si>
-    <t>R40, R41, R42, R45, R46, R47</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
     <t>R43, R44, R59, R60</t>
   </si>
   <si>
@@ -468,10 +483,10 @@
     <t>Thermistor_PTC</t>
   </si>
   <si>
-    <t>Fuse:Fuse_0603_1608Metric_Pad1.05x0.95mm_HandSolder</t>
-  </si>
-  <si>
-    <t>PRG18BC1R0MM1RB</t>
+    <t>Fuse:Fuse_1206_3216Metric</t>
+  </si>
+  <si>
+    <t>ASMD1206-100</t>
   </si>
   <si>
     <t>U1</t>
@@ -501,15 +516,6 @@
     <t>MACHADA_footprints:A9G_MODULE</t>
   </si>
   <si>
-    <t>U4, U6, U10, U12, U18, U20</t>
-  </si>
-  <si>
-    <t>TBU-CA065-200-WH</t>
-  </si>
-  <si>
-    <t>MACHADA_footprints:TBU-CA065-200-WH</t>
-  </si>
-  <si>
     <t>U5, U11, U19</t>
   </si>
   <si>
@@ -522,7 +528,7 @@
     <t>U7, U14</t>
   </si>
   <si>
-    <t>WAS3157B</t>
+    <t>SN74LVC1G3157DBVR</t>
   </si>
   <si>
     <t>Package_TO_SOT_SMD:SOT-363_SC-70-6</t>
@@ -591,9 +597,6 @@
     <t>Q13FC1350000200</t>
   </si>
   <si>
-    <t>Vendor</t>
-  </si>
-  <si>
     <t>2337019-1</t>
   </si>
   <si>
@@ -642,10 +645,10 @@
     <t>SP0504BAHTG</t>
   </si>
   <si>
-    <t>ZX-NSIM-281.4J</t>
-  </si>
-  <si>
-    <t>BLM18BD421SH1D</t>
+    <t>BZT52C4V3</t>
+  </si>
+  <si>
+    <t>BLM15HD182SN1D</t>
   </si>
   <si>
     <t>SDCL1005C82NJTDF</t>
@@ -675,15 +678,15 @@
     <t>RC0402JR-074K7L</t>
   </si>
   <si>
+    <t>RC0402FR-0722RL</t>
+  </si>
+  <si>
     <t>RC0402FR-7W1KL</t>
   </si>
   <si>
     <t>RC0402FR-072K2L</t>
   </si>
   <si>
-    <t>RC0402FR-0722RL</t>
-  </si>
-  <si>
     <t>RC0402FR-07200KL</t>
   </si>
   <si>
@@ -709,9 +712,6 @@
   </si>
   <si>
     <t>A9G</t>
-  </si>
-  <si>
-    <t>WAS3157B-6/TR</t>
   </si>
   <si>
     <t>W25Q32JVSSIQ</t>
@@ -730,7 +730,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -865,14 +865,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -1177,7 +1169,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1220,17 +1212,15 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1264,7 +1254,6 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1585,52 +1574,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F74"/>
+  <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E74"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13.21875" customWidth="1"/>
-    <col min="3" max="3" width="51" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.77734375" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="32.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
         <v>232</v>
@@ -1641,36 +1630,36 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>189</v>
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="E3" t="s">
         <v>232</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E4" t="s">
         <v>232</v>
@@ -1681,16 +1670,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>191</v>
+        <v>17</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="E5" t="s">
         <v>232</v>
@@ -1701,16 +1690,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>192</v>
+      <c r="D6" s="2" t="s">
+        <v>193</v>
       </c>
       <c r="E6" t="s">
         <v>232</v>
@@ -1721,16 +1710,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>193</v>
+        <v>17</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>194</v>
       </c>
       <c r="E7" t="s">
         <v>232</v>
@@ -1741,16 +1730,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>194</v>
+        <v>17</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>195</v>
       </c>
       <c r="E8" t="s">
         <v>232</v>
@@ -1761,16 +1750,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E9" t="s">
         <v>232</v>
@@ -1781,16 +1770,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>192</v>
+        <v>17</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>193</v>
       </c>
       <c r="E10" t="s">
         <v>232</v>
@@ -1801,16 +1790,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="E11" t="s">
         <v>232</v>
@@ -1821,33 +1807,33 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
         <v>30</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>31</v>
       </c>
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
       <c r="D12" t="s">
-        <v>195</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s">
         <v>232</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
         <v>196</v>
@@ -1867,7 +1853,7 @@
         <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s">
         <v>197</v>
@@ -1881,13 +1867,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
         <v>37</v>
-      </c>
-      <c r="B15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" t="s">
-        <v>34</v>
       </c>
       <c r="D15" t="s">
         <v>198</v>
@@ -1901,13 +1887,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
         <v>199</v>
@@ -1921,13 +1907,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D17" t="s">
         <v>200</v>
@@ -1936,27 +1922,27 @@
         <v>232</v>
       </c>
       <c r="F17">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
+        <v>201</v>
       </c>
       <c r="E18" t="s">
         <v>232</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1969,8 +1955,8 @@
       <c r="C19" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>201</v>
+      <c r="D19" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="E19" t="s">
         <v>232</v>
@@ -1989,8 +1975,8 @@
       <c r="C20" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>49</v>
+      <c r="D20" s="2" t="s">
+        <v>202</v>
       </c>
       <c r="E20" t="s">
         <v>232</v>
@@ -2009,8 +1995,8 @@
       <c r="C21" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>202</v>
+      <c r="D21" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="E21" t="s">
         <v>232</v>
@@ -2029,7 +2015,7 @@
       <c r="C22" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="2" t="s">
         <v>203</v>
       </c>
       <c r="E22" t="s">
@@ -2047,9 +2033,9 @@
         <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>204</v>
       </c>
       <c r="E23" t="s">
@@ -2067,16 +2053,16 @@
         <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>60</v>
+        <v>50</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>205</v>
       </c>
       <c r="E24" t="s">
         <v>232</v>
       </c>
       <c r="F24">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -2087,56 +2073,56 @@
         <v>62</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E25" t="s">
         <v>232</v>
       </c>
       <c r="F25">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" t="s">
         <v>64</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>65</v>
       </c>
-      <c r="C26" t="s">
-        <v>66</v>
-      </c>
       <c r="D26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E26" t="s">
         <v>232</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" t="s">
         <v>67</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>68</v>
       </c>
-      <c r="C27" t="s">
-        <v>66</v>
-      </c>
       <c r="D27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E27" t="s">
         <v>232</v>
       </c>
       <c r="F27">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -2147,10 +2133,10 @@
         <v>70</v>
       </c>
       <c r="C28" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="D28" t="s">
-        <v>70</v>
+        <v>206</v>
       </c>
       <c r="E28" t="s">
         <v>232</v>
@@ -2161,16 +2147,16 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" t="s">
         <v>72</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>73</v>
       </c>
-      <c r="C29" t="s">
-        <v>74</v>
-      </c>
       <c r="D29" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E29" t="s">
         <v>232</v>
@@ -2181,16 +2167,16 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" t="s">
         <v>76</v>
       </c>
-      <c r="B30" t="s">
+      <c r="D30" t="s">
         <v>77</v>
-      </c>
-      <c r="C30" t="s">
-        <v>78</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>205</v>
       </c>
       <c r="E30" t="s">
         <v>232</v>
@@ -2201,16 +2187,16 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" t="s">
         <v>79</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>80</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>81</v>
-      </c>
-      <c r="D31">
-        <v>5033981892</v>
       </c>
       <c r="E31" t="s">
         <v>232</v>
@@ -2229,8 +2215,8 @@
       <c r="C32" t="s">
         <v>84</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>206</v>
+      <c r="D32">
+        <v>5033981892</v>
       </c>
       <c r="E32" t="s">
         <v>232</v>
@@ -2267,10 +2253,10 @@
         <v>89</v>
       </c>
       <c r="C34" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D34" t="s">
-        <v>91</v>
+        <v>208</v>
       </c>
       <c r="E34" t="s">
         <v>232</v>
@@ -2281,33 +2267,33 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B35" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C35" t="s">
-        <v>63</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
+      </c>
+      <c r="D35" t="s">
+        <v>207</v>
       </c>
       <c r="E35" t="s">
         <v>232</v>
       </c>
       <c r="F35">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36" t="s">
         <v>94</v>
-      </c>
-      <c r="B36" t="s">
-        <v>95</v>
-      </c>
-      <c r="C36" t="s">
-        <v>63</v>
       </c>
       <c r="D36" t="s">
         <v>95</v>
@@ -2324,13 +2310,13 @@
         <v>96</v>
       </c>
       <c r="B37" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C37" t="s">
-        <v>63</v>
-      </c>
-      <c r="D37" t="s">
-        <v>95</v>
+        <v>65</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="E37" t="s">
         <v>232</v>
@@ -2341,16 +2327,16 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B38" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C38" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" t="s">
         <v>99</v>
-      </c>
-      <c r="D38" t="s">
-        <v>208</v>
       </c>
       <c r="E38" t="s">
         <v>232</v>
@@ -2364,39 +2350,39 @@
         <v>100</v>
       </c>
       <c r="B39" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C39" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" t="s">
         <v>99</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="E39" t="s">
         <v>232</v>
       </c>
       <c r="F39">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>101</v>
+      </c>
+      <c r="B40" t="s">
         <v>102</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>103</v>
       </c>
-      <c r="C40" t="s">
-        <v>99</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>210</v>
+      <c r="D40" t="s">
+        <v>209</v>
       </c>
       <c r="E40" t="s">
         <v>232</v>
       </c>
       <c r="F40">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -2407,16 +2393,16 @@
         <v>105</v>
       </c>
       <c r="C41" t="s">
-        <v>99</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>211</v>
+        <v>103</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>210</v>
       </c>
       <c r="E41" t="s">
         <v>232</v>
       </c>
       <c r="F41">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -2427,16 +2413,16 @@
         <v>107</v>
       </c>
       <c r="C42" t="s">
-        <v>99</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>212</v>
+        <v>103</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="E42" t="s">
         <v>232</v>
       </c>
       <c r="F42">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -2447,16 +2433,16 @@
         <v>109</v>
       </c>
       <c r="C43" t="s">
-        <v>99</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>213</v>
+        <v>103</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>212</v>
       </c>
       <c r="E43" t="s">
         <v>232</v>
       </c>
       <c r="F43">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -2467,16 +2453,16 @@
         <v>111</v>
       </c>
       <c r="C44" t="s">
-        <v>99</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>214</v>
+        <v>103</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>213</v>
       </c>
       <c r="E44" t="s">
         <v>232</v>
       </c>
       <c r="F44">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -2487,16 +2473,16 @@
         <v>113</v>
       </c>
       <c r="C45" t="s">
-        <v>99</v>
-      </c>
-      <c r="D45" t="s">
-        <v>215</v>
+        <v>103</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="E45" t="s">
         <v>232</v>
       </c>
       <c r="F45">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -2507,16 +2493,16 @@
         <v>115</v>
       </c>
       <c r="C46" t="s">
-        <v>99</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>216</v>
+        <v>103</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>215</v>
       </c>
       <c r="E46" t="s">
         <v>232</v>
       </c>
       <c r="F46">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -2524,13 +2510,13 @@
         <v>116</v>
       </c>
       <c r="B47" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="C47" t="s">
-        <v>99</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>213</v>
+        <v>103</v>
+      </c>
+      <c r="D47" t="s">
+        <v>216</v>
       </c>
       <c r="E47" t="s">
         <v>232</v>
@@ -2541,96 +2527,96 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B48" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C48" t="s">
-        <v>99</v>
-      </c>
-      <c r="D48" t="s">
+        <v>103</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>217</v>
       </c>
       <c r="E48" t="s">
         <v>232</v>
       </c>
       <c r="F48">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B49" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C49" t="s">
-        <v>99</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>218</v>
+        <v>103</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="E49" t="s">
         <v>232</v>
       </c>
       <c r="F49">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B50" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C50" t="s">
-        <v>99</v>
-      </c>
-      <c r="D50" t="s">
-        <v>219</v>
+        <v>103</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>218</v>
       </c>
       <c r="E50" t="s">
         <v>232</v>
       </c>
       <c r="F50">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B51" t="s">
+        <v>105</v>
+      </c>
+      <c r="C51" t="s">
         <v>103</v>
       </c>
-      <c r="C51" t="s">
-        <v>99</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>210</v>
+      <c r="D51" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="E51" t="s">
         <v>232</v>
       </c>
       <c r="F51">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B52" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C52" t="s">
-        <v>99</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>220</v>
+        <v>103</v>
+      </c>
+      <c r="D52" t="s">
+        <v>219</v>
       </c>
       <c r="E52" t="s">
         <v>232</v>
@@ -2641,22 +2627,22 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B53" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C53" t="s">
-        <v>99</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>209</v>
+        <v>103</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>217</v>
       </c>
       <c r="E53" t="s">
         <v>232</v>
       </c>
       <c r="F53">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -2667,16 +2653,16 @@
         <v>129</v>
       </c>
       <c r="C54" t="s">
-        <v>99</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>221</v>
+        <v>103</v>
+      </c>
+      <c r="D54" t="s">
+        <v>220</v>
       </c>
       <c r="E54" t="s">
         <v>232</v>
       </c>
       <c r="F54">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -2684,13 +2670,13 @@
         <v>130</v>
       </c>
       <c r="B55" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="C55" t="s">
-        <v>99</v>
-      </c>
-      <c r="D55" t="s">
-        <v>222</v>
+        <v>103</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="E55" t="s">
         <v>232</v>
@@ -2701,22 +2687,22 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>131</v>
+      </c>
+      <c r="B56" t="s">
         <v>132</v>
       </c>
-      <c r="B56" t="s">
-        <v>115</v>
-      </c>
       <c r="C56" t="s">
-        <v>99</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>216</v>
+        <v>103</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>221</v>
       </c>
       <c r="E56" t="s">
         <v>232</v>
       </c>
       <c r="F56">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -2727,16 +2713,16 @@
         <v>134</v>
       </c>
       <c r="C57" t="s">
-        <v>99</v>
-      </c>
-      <c r="D57" t="s">
-        <v>223</v>
+        <v>103</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>222</v>
       </c>
       <c r="E57" t="s">
         <v>232</v>
       </c>
       <c r="F57">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -2747,10 +2733,10 @@
         <v>136</v>
       </c>
       <c r="C58" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D58" t="s">
-        <v>137</v>
+        <v>223</v>
       </c>
       <c r="E58" t="s">
         <v>232</v>
@@ -2761,16 +2747,16 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B59" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="C59" t="s">
-        <v>140</v>
-      </c>
-      <c r="D59" t="s">
-        <v>141</v>
+        <v>103</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>218</v>
       </c>
       <c r="E59" t="s">
         <v>232</v>
@@ -2781,13 +2767,13 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B60" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C60" t="s">
-        <v>144</v>
+        <v>103</v>
       </c>
       <c r="D60" t="s">
         <v>224</v>
@@ -2801,16 +2787,16 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B61" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C61" t="s">
-        <v>147</v>
+        <v>103</v>
       </c>
       <c r="D61" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="E61" t="s">
         <v>232</v>
@@ -2821,16 +2807,16 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B62" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C62" t="s">
-        <v>151</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>225</v>
+        <v>145</v>
+      </c>
+      <c r="D62" t="s">
+        <v>146</v>
       </c>
       <c r="E62" t="s">
         <v>232</v>
@@ -2841,16 +2827,16 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B63" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C63" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D63" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E63" t="s">
         <v>232</v>
@@ -2861,16 +2847,16 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B64" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C64" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D64" t="s">
-        <v>227</v>
+        <v>153</v>
       </c>
       <c r="E64" t="s">
         <v>232</v>
@@ -2881,53 +2867,53 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B65" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C65" t="s">
-        <v>160</v>
-      </c>
-      <c r="D65" t="s">
-        <v>159</v>
+        <v>156</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>226</v>
       </c>
       <c r="E65" t="s">
         <v>232</v>
       </c>
       <c r="F65">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B66" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C66" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D66" t="s">
-        <v>162</v>
+        <v>227</v>
       </c>
       <c r="E66" t="s">
         <v>232</v>
       </c>
       <c r="F66">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B67" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C67" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D67" t="s">
         <v>228</v>
@@ -2936,41 +2922,41 @@
         <v>232</v>
       </c>
       <c r="F67">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B68" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C68" t="s">
-        <v>169</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>229</v>
+        <v>165</v>
+      </c>
+      <c r="D68" t="s">
+        <v>164</v>
       </c>
       <c r="E68" t="s">
         <v>232</v>
       </c>
       <c r="F68">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B69" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C69" t="s">
-        <v>172</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
+      </c>
+      <c r="D69" t="s">
+        <v>167</v>
       </c>
       <c r="E69" t="s">
         <v>232</v>
@@ -2981,16 +2967,16 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B70" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C70" t="s">
-        <v>175</v>
-      </c>
-      <c r="D70" t="s">
-        <v>174</v>
+        <v>171</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>229</v>
       </c>
       <c r="E70" t="s">
         <v>232</v>
@@ -3001,36 +2987,36 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B71" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C71" t="s">
-        <v>53</v>
-      </c>
-      <c r="D71" t="s">
-        <v>177</v>
+        <v>174</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="E71" t="s">
         <v>232</v>
       </c>
       <c r="F71">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B72" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C72" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D72" t="s">
-        <v>230</v>
+        <v>176</v>
       </c>
       <c r="E72" t="s">
         <v>232</v>
@@ -3041,16 +3027,16 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B73" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C73" t="s">
-        <v>183</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>231</v>
+        <v>56</v>
+      </c>
+      <c r="D73" t="s">
+        <v>179</v>
       </c>
       <c r="E73" t="s">
         <v>232</v>
@@ -3061,29 +3047,65 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
+        <v>180</v>
+      </c>
+      <c r="B74" t="s">
+        <v>181</v>
+      </c>
+      <c r="C74" t="s">
+        <v>182</v>
+      </c>
+      <c r="D74" t="s">
+        <v>230</v>
+      </c>
+      <c r="E74" t="s">
+        <v>232</v>
+      </c>
+      <c r="F74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>183</v>
+      </c>
+      <c r="B75" t="s">
         <v>184</v>
       </c>
-      <c r="B74" t="s">
+      <c r="C75" t="s">
         <v>185</v>
       </c>
-      <c r="C74" t="s">
+      <c r="D75" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="E75" t="s">
+        <v>232</v>
+      </c>
+      <c r="F75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
         <v>186</v>
       </c>
-      <c r="D74" t="s">
+      <c r="B76" t="s">
         <v>187</v>
       </c>
-      <c r="E74" t="s">
-        <v>232</v>
-      </c>
-      <c r="F74">
+      <c r="C76" t="s">
+        <v>188</v>
+      </c>
+      <c r="D76" t="s">
+        <v>189</v>
+      </c>
+      <c r="E76" t="s">
+        <v>232</v>
+      </c>
+      <c r="F76">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D30" r:id="rId1" display="https://www.lcsc.com/product-detail/span-style-background-color-ff0-SIM-span-Card-Connectors_Megastar-ZX-NSIM-281-4J_C7419853.html"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>